<commit_message>
EPBDS Rules loader accessing through a static methods instead of setting fields of Data table.
</commit_message>
<xml_diff>
--- a/WSFrontend/trunk/org.openl.rules.ruleservice/src/RulesBasedConfigurerTemplate.xlsx
+++ b/WSFrontend/trunk/org.openl.rules.ruleservice/src/RulesBasedConfigurerTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="9345" windowHeight="3195" activeTab="1"/>
+    <workbookView xWindow="285" yWindow="105" windowWidth="9345" windowHeight="3195"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>import</t>
   </si>
@@ -37,21 +37,9 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>Data IRulesLoader loader</t>
-  </si>
-  <si>
     <t>org.openl.rules.project.abstraction</t>
   </si>
   <si>
-    <t>deploymentName</t>
-  </si>
-  <si>
-    <t>dataSource</t>
-  </si>
-  <si>
-    <t>Data Deployment deployments</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -127,11 +115,128 @@
     <t>Method CommonVersion getLastVersion(String deplName)</t>
   </si>
   <si>
-    <t>Method List getAutoModules()</t>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Service URL</t>
+  </si>
+  <si>
+    <t>Service interface</t>
+  </si>
+  <si>
+    <t>Provide runtime context</t>
+  </si>
+  <si>
+    <t>org.openl.rules.project.model</t>
+  </si>
+  <si>
+    <t>Datatype  Service</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Data Service services</t>
+  </si>
+  <si>
+    <t>modulesGetter</t>
+  </si>
+  <si>
+    <t>Method returning modules for service</t>
+  </si>
+  <si>
+    <t>getAutoModules</t>
+  </si>
+  <si>
+    <t>Method List getModules(String deploymentName, CommonVersion deploymentVersion, String projectName, String[] moduleNames)</t>
+  </si>
+  <si>
+    <t>Rules List getModulesForAutoDeployment(Deployment deployment, String project)</t>
+  </si>
+  <si>
+    <t>String projectName</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>=getAllModulesForProject(deployment.deploymentName, deployment.commonVersion, project)</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Deploymen Name</t>
+  </si>
+  <si>
+    <t>Deployment Version</t>
+  </si>
+  <si>
+    <t>Project In The Deployment</t>
+  </si>
+  <si>
+    <t>Method IRulesLoader getLoader()</t>
+  </si>
+  <si>
+    <t>return RulesBasedServiceConfigurer.getLoader();</t>
+  </si>
+  <si>
+    <t>Method Deployment[] getDeployments()</t>
+  </si>
+  <si>
+    <t>return RulesBasedServiceConfigurer.getDeployments();</t>
+  </si>
+  <si>
+    <t>Method List getModules()</t>
+  </si>
+  <si>
+    <t>List modules = new ArrayList();
+for(int i=0; i&lt; getDeployments().length; i++){
+  AProject[] projects = new AProject[getDeployments()[i].projects.size()];
+  projects = (AProject[])getDeployments()[i].projects.toArray(projects);
+  for(int j=0; j&lt;projects.length; j++) {
+    List appropriateModules = getModulesForDeployment(getDeployments()[i], projects[j].name);
+    if(appropriateModules != null) {
+      modules.addAll(appropriateModules);
+    }
+  }
+}
+return modules;</t>
+  </si>
+  <si>
+    <t>List modules = new ArrayList();
+Deployment deployment = getLoader().getDeployment(deploymentName, deploymentVersion);
+AProject[] projects = new AProject[deployment.projects.size()];
+projects = (AProject[])deployment.projects.toArray(projects);
+for(int i=0; i&lt; projects.length; i++){
+  modules.addAll(getAllModulesForProject(deploymentName,deploymentVersion, projects[i].name));
+}
+return modules;</t>
+  </si>
+  <si>
+    <t>List moduleConfigurations = new ArrayList();
+List modules = getLoader().resolveModulesForProject(deploymentName,deploymentVersion, projectName);
+for(int i=0; i&lt;modules.size(); i++){
+  moduleConfigurations.add(new ModuleConfiguration(deploymentName, deploymentVersion, projectName, ((Module)modules.get(i)).name));
+}
+return moduleConfigurations;</t>
+  </si>
+  <si>
+    <t>List moduleConfigurations = new ArrayList();
+List modules = getLoader().resolveModulesForProject(deploymentName,deploymentVersion, projectName);
+for(int i=0; i&lt;modules.size(); i++){
+  if (contains(moduleNames, ((Module)modules.get(i)).name)) {
+    moduleConfigurations.add(new ModuleConfiguration(deploymentName, deploymentVersion, projectName, ((Module)modules.get(i)).name));
+  }
+}
+return moduleConfigurations;</t>
   </si>
   <si>
     <t>CommonVersion lastVersion = null;
-Deployment[] applicableDeployments = deployments[@deploymentName == deplName];
+Deployment[] applicableDeployments = getDeployments()[@deploymentName == deplName];
 for(int i=0; i &lt; applicableDeployments.length; i++){
   if(lastVersion == null || lastVersion.compareTo(applicableDeployments[i].commonVersion) &lt; 0){
     lastVersion = applicableDeployments[i].commonVersion;
@@ -140,109 +245,7 @@
 return lastVersion;</t>
   </si>
   <si>
-    <t>List modules = new ArrayList();
-Deployment deployment = loader[0].getDeployment(deploymentName, deploymentVersion);
-AProject[] projects = new AProject[deployment.projects.size()];
-projects = (AProject[])deployment.projects.toArray(projects);
-for(int i=0; i&lt; projects.length; i++){
-  modules.addAll(getAllModulesForProject(deploymentName,deploymentVersion, projects[i].name));
-}
-return modules;</t>
-  </si>
-  <si>
-    <t>Service Name</t>
-  </si>
-  <si>
-    <t>Service URL</t>
-  </si>
-  <si>
-    <t>Service interface</t>
-  </si>
-  <si>
-    <t>Provide runtime context</t>
-  </si>
-  <si>
-    <t>List moduleConfigurations = new ArrayList();
-List modules = loader[0].resolveModulesForProject(deploymentName,deploymentVersion, projectName);
-for(int i=0; i&lt;modules.size(); i++){
-  moduleConfigurations.add(new ModuleConfiguration(deploymentName, deploymentVersion, projectName, ((Module)modules.get(i)).name));
-}
-return moduleConfigurations;</t>
-  </si>
-  <si>
-    <t>org.openl.rules.project.model</t>
-  </si>
-  <si>
-    <t>Datatype  Service</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>Data Service services</t>
-  </si>
-  <si>
-    <t>modulesGetter</t>
-  </si>
-  <si>
-    <t>Method returning modules for service</t>
-  </si>
-  <si>
-    <t>getAutoModules</t>
-  </si>
-  <si>
-    <t>Method List getModules(String deploymentName, CommonVersion deploymentVersion, String projectName, String[] moduleNames)</t>
-  </si>
-  <si>
-    <t>Rules List getModulesForAutoDeployment(Deployment deployment, String project)</t>
-  </si>
-  <si>
-    <t>String projectName</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>=getAllModulesForProject(deployment.deploymentName, deployment.commonVersion, project)</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>List moduleConfigurations = new ArrayList();
-List modules = loader[0].resolveModulesForProject(deploymentName,deploymentVersion, projectName);
-for(int i=0; i&lt;modules.size(); i++){
-  if (contains(moduleNames, ((Module)modules.get(i)).name)) {
-    moduleConfigurations.add(new ModuleConfiguration(deploymentName, deploymentVersion, projectName, ((Module)modules.get(i)).name));
-  }
-}
-return moduleConfigurations;</t>
-  </si>
-  <si>
-    <t>List modules = new ArrayList();
-for(int i=0; i&lt; deployments.length; i++){
-  AProject[] projects = new AProject[deployments[i].projects.size()];
-  projects = (AProject[])deployments[i].projects.toArray(projects);
-  for(int j=0; j&lt;projects.length; j++) {
-    List appropriateModules = getModulesForAutoDeployment(deployments[i], projects[j].name);
-    if(appropriateModules != null) {
-      modules.addAll(appropriateModules);
-    }
-  }
-}
-return modules;</t>
-  </si>
-  <si>
-    <t>Deploymen Name</t>
-  </si>
-  <si>
-    <t>Deployment Version</t>
-  </si>
-  <si>
-    <t>Project In The Deployment</t>
+    <t>org.openl.rules.ruleservice.management</t>
   </si>
 </sst>
 </file>
@@ -336,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -558,19 +561,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -616,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -670,33 +660,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -704,23 +672,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,9 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1154,147 +1141,151 @@
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
+    <row r="2" spans="2:4">
+      <c r="B2" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="32"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="2:4">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="34" t="s">
-        <v>4</v>
-      </c>
+      <c r="B17" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="36" t="s">
-        <v>7</v>
-      </c>
+      <c r="B18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
+      <c r="B19" s="1"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
+      <c r="B22" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="17"/>
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7" ht="12.75" customHeight="1">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>40</v>
+      <c r="B26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>48</v>
+      <c r="B27" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -1304,9 +1295,13 @@
       <c r="D31" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1316,9 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1330,124 +1323,124 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="12" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="16"/>
       <c r="C8" s="19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="39"/>
+      <c r="B11" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="35"/>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="2:5" ht="153" customHeight="1">
-      <c r="B12" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="38"/>
+      <c r="B12" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="30"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1471,9 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1484,18 +1475,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B4" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
+      <c r="B4" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" ht="132" customHeight="1">
-      <c r="B5" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
+      <c r="B5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1"/>
@@ -1503,18 +1494,18 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B7" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
     </row>
     <row r="8" spans="2:4" ht="105" customHeight="1">
-      <c r="B8" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
+      <c r="B8" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="1"/>
@@ -1527,18 +1518,18 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B11" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
     </row>
     <row r="12" spans="2:4" ht="128.25" customHeight="1">
-      <c r="B12" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
+      <c r="B12" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="1"/>
@@ -1551,29 +1542,29 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="12.75" customHeight="1">
-      <c r="B15" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="B15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
     </row>
     <row r="16" spans="2:4" ht="112.5" customHeight="1">
-      <c r="B16" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
+      <c r="B16" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1581,23 +1572,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="42" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1605,33 +1596,39 @@
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="26"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="26"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="26"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="26"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="43"/>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B3:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing framework improvements. Refactoring. JavaDocs.
</commit_message>
<xml_diff>
--- a/WSFrontend/trunk/org.openl.rules.ruleservice/src/RulesBasedConfigurerTemplate.xlsx
+++ b/WSFrontend/trunk/org.openl.rules.ruleservice/src/RulesBasedConfigurerTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="9345" windowHeight="3195"/>
+    <workbookView xWindow="285" yWindow="105" windowWidth="9345" windowHeight="3195" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="6" r:id="rId1"/>
@@ -162,9 +162,6 @@
 return lastVersion;</t>
   </si>
   <si>
-    <t>org.openl.rules.ruleservice.management</t>
-  </si>
-  <si>
     <t>Rules boolean modulesForAuto(Deployment deployment, AProject project, Module module)</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Method RuleServiceLoader getLoader()</t>
+  </si>
+  <si>
+    <t>org.openl.rules.ruleservice.conf</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
@@ -1289,7 +1289,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>32</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="48"/>
       <c r="D2" s="29"/>
@@ -1368,13 +1368,13 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -1465,15 +1465,15 @@
   <sheetData>
     <row r="2" spans="2:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
@@ -1495,16 +1495,16 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -1533,13 +1533,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="18" t="b">
         <v>1</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>18</v>
@@ -1572,15 +1572,15 @@
     </row>
     <row r="13" spans="2:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -1602,16 +1602,16 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1620,10 +1620,10 @@
         <v>33</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="35"/>
       <c r="C19" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="18" t="b">
@@ -1654,7 +1654,7 @@
       <c r="B20" s="36"/>
       <c r="C20" s="17"/>
       <c r="D20" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="18" t="b">
         <v>1</v>
@@ -1667,12 +1667,12 @@
     </row>
     <row r="23" spans="2:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B23" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
@@ -1698,19 +1698,19 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
@@ -1720,10 +1720,10 @@
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1737,7 +1737,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>8</v>
@@ -1745,13 +1745,13 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="34"/>
       <c r="F29" s="18" t="b">
@@ -1763,7 +1763,7 @@
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F30" s="18" t="b">
         <v>1</v>
@@ -1843,7 +1843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1891,7 +1893,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="52"/>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>